<commit_message>
minor fixes in the json
</commit_message>
<xml_diff>
--- a/excelReader.xlsx
+++ b/excelReader.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yarde\PycharmProjects\pythonProject\evolutionary_algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1036C12-DF8D-40AC-821B-D3AB8E116F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E3B49E-93D4-4F88-AD21-2F28108547EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6675" yWindow="2595" windowWidth="21600" windowHeight="11385" xr2:uid="{00FC73E2-83E3-40DE-89D7-9490E3BC3A17}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00FC73E2-83E3-40DE-89D7-9490E3BC3A17}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4126" uniqueCount="2685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4125" uniqueCount="2684">
   <si>
     <t>Code</t>
   </si>
@@ -7920,9 +7920,6 @@
   </si>
   <si>
     <t>0.6</t>
-  </si>
-  <si>
-    <t>tr</t>
   </si>
   <si>
     <t>26.1</t>
@@ -8718,8 +8715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC99E6F-A577-43BC-955A-BE0EB99AA943}">
   <dimension ref="A1:F1029"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A939" workbookViewId="0">
+      <selection activeCell="D952" sqref="D952"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8735,7 +8732,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2684</v>
+        <v>2683</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>505</v>
@@ -8744,10 +8741,10 @@
         <v>506</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>2681</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2682</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>2683</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="36" x14ac:dyDescent="0.25">
@@ -9327,7 +9324,7 @@
         <v>528</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>2660</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="36" x14ac:dyDescent="0.25">
@@ -9467,7 +9464,7 @@
         <v>147</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -9567,7 +9564,7 @@
         <v>519</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -10467,7 +10464,7 @@
         <v>561</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -10607,7 +10604,7 @@
         <v>558</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -10647,7 +10644,7 @@
         <v>567</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -10930,7 +10927,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A111" s="38" t="s">
         <v>344</v>
       </c>
@@ -11027,7 +11024,7 @@
         <v>271</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -11047,7 +11044,7 @@
         <v>553</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -11147,7 +11144,7 @@
         <v>575</v>
       </c>
       <c r="F121" s="4" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -11167,7 +11164,7 @@
         <v>575</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -11310,7 +11307,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A130" s="38" t="s">
         <v>385</v>
       </c>
@@ -12487,7 +12484,7 @@
         <v>80</v>
       </c>
       <c r="F188" s="20" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="189" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -14347,7 +14344,7 @@
         <v>604</v>
       </c>
       <c r="F281" s="20" t="s">
-        <v>2661</v>
+        <v>2660</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.25">
@@ -14547,7 +14544,7 @@
         <v>14.5</v>
       </c>
       <c r="F291" s="20" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="292" spans="1:6" x14ac:dyDescent="0.25">
@@ -14567,7 +14564,7 @@
         <v>7.5</v>
       </c>
       <c r="F292" s="20" t="s">
-        <v>2662</v>
+        <v>2661</v>
       </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.25">
@@ -15667,7 +15664,7 @@
         <v>19</v>
       </c>
       <c r="F347" s="20" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="348" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -15707,7 +15704,7 @@
         <v>19</v>
       </c>
       <c r="F349" s="20" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="350" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -15887,7 +15884,7 @@
         <v>10.5</v>
       </c>
       <c r="F358" s="20" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="359" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -15927,7 +15924,7 @@
         <v>10.5</v>
       </c>
       <c r="F360" s="20" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="361" spans="1:6" x14ac:dyDescent="0.25">
@@ -16747,7 +16744,7 @@
         <v>12.1</v>
       </c>
       <c r="F401" s="20" t="s">
-        <v>2663</v>
+        <v>2662</v>
       </c>
     </row>
     <row r="402" spans="1:6" x14ac:dyDescent="0.25">
@@ -17107,7 +17104,7 @@
         <v>3.2</v>
       </c>
       <c r="F419" s="6" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="420" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -18327,7 +18324,7 @@
         <v>4.8</v>
       </c>
       <c r="F480" s="6" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="481" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -18627,7 +18624,7 @@
         <v>6.4</v>
       </c>
       <c r="F495" s="6" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="496" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -18647,7 +18644,7 @@
         <v>6.4</v>
       </c>
       <c r="F496" s="6" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="497" spans="1:6" x14ac:dyDescent="0.25">
@@ -19047,7 +19044,7 @@
         <v>0.9</v>
       </c>
       <c r="F516" s="6" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="517" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -19327,7 +19324,7 @@
         <v>13.6</v>
       </c>
       <c r="F530" s="6" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="531" spans="1:6" x14ac:dyDescent="0.25">
@@ -19827,7 +19824,7 @@
         <v>36</v>
       </c>
       <c r="F555" s="6" t="s">
-        <v>2660</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="556" spans="1:6" x14ac:dyDescent="0.25">
@@ -19847,7 +19844,7 @@
         <v>12.1</v>
       </c>
       <c r="F556" s="6" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="557" spans="1:6" x14ac:dyDescent="0.25">
@@ -19947,7 +19944,7 @@
         <v>24.9</v>
       </c>
       <c r="F561" s="6" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="562" spans="1:6" x14ac:dyDescent="0.25">
@@ -20527,7 +20524,7 @@
         <v>614</v>
       </c>
       <c r="F590" s="6" t="s">
-        <v>2664</v>
+        <v>2663</v>
       </c>
     </row>
     <row r="591" spans="1:6" x14ac:dyDescent="0.25">
@@ -20807,7 +20804,7 @@
         <v>17.100000000000001</v>
       </c>
       <c r="F604" s="6" t="s">
-        <v>2665</v>
+        <v>2664</v>
       </c>
     </row>
     <row r="605" spans="1:6" x14ac:dyDescent="0.25">
@@ -20887,7 +20884,7 @@
         <v>14.2</v>
       </c>
       <c r="F608" s="6" t="s">
-        <v>2666</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="609" spans="1:6" x14ac:dyDescent="0.25">
@@ -21027,7 +21024,7 @@
         <v>20.399999999999999</v>
       </c>
       <c r="F615" s="6" t="s">
-        <v>2667</v>
+        <v>2666</v>
       </c>
     </row>
     <row r="616" spans="1:6" x14ac:dyDescent="0.25">
@@ -21087,7 +21084,7 @@
         <v>11</v>
       </c>
       <c r="F618" s="6" t="s">
-        <v>2668</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="619" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -21107,7 +21104,7 @@
         <v>23.2</v>
       </c>
       <c r="F619" s="6" t="s">
-        <v>2669</v>
+        <v>2668</v>
       </c>
     </row>
     <row r="620" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -21127,7 +21124,7 @@
         <v>14.7</v>
       </c>
       <c r="F620" s="6" t="s">
-        <v>2670</v>
+        <v>2669</v>
       </c>
     </row>
     <row r="621" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -21147,7 +21144,7 @@
         <v>10.4</v>
       </c>
       <c r="F621" s="6" t="s">
-        <v>2671</v>
+        <v>2670</v>
       </c>
     </row>
     <row r="622" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -21167,7 +21164,7 @@
         <v>17.600000000000001</v>
       </c>
       <c r="F622" s="6" t="s">
-        <v>2672</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="623" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -21187,7 +21184,7 @@
         <v>11.7</v>
       </c>
       <c r="F623" s="6" t="s">
-        <v>2673</v>
+        <v>2672</v>
       </c>
     </row>
     <row r="624" spans="1:6" x14ac:dyDescent="0.25">
@@ -21307,7 +21304,7 @@
         <v>19</v>
       </c>
       <c r="F629" s="6" t="s">
-        <v>2674</v>
+        <v>2673</v>
       </c>
     </row>
     <row r="630" spans="1:6" x14ac:dyDescent="0.25">
@@ -21347,7 +21344,7 @@
         <v>29</v>
       </c>
       <c r="F631" s="6" t="s">
-        <v>2675</v>
+        <v>2674</v>
       </c>
     </row>
     <row r="632" spans="1:6" x14ac:dyDescent="0.25">
@@ -21367,7 +21364,7 @@
         <v>12.6</v>
       </c>
       <c r="F632" s="6" t="s">
-        <v>2676</v>
+        <v>2675</v>
       </c>
     </row>
     <row r="633" spans="1:6" x14ac:dyDescent="0.25">
@@ -21447,7 +21444,7 @@
         <v>34.1</v>
       </c>
       <c r="F636" s="6" t="s">
-        <v>2677</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="637" spans="1:6" x14ac:dyDescent="0.25">
@@ -21467,7 +21464,7 @@
         <v>615</v>
       </c>
       <c r="F637" s="16" t="s">
-        <v>2678</v>
+        <v>2677</v>
       </c>
     </row>
     <row r="638" spans="1:6" x14ac:dyDescent="0.25">
@@ -21478,7 +21475,7 @@
         <v>2168</v>
       </c>
       <c r="C638" s="16" t="s">
-        <v>2679</v>
+        <v>2678</v>
       </c>
       <c r="D638" s="16" t="s">
         <v>593</v>
@@ -21487,7 +21484,7 @@
         <v>211</v>
       </c>
       <c r="F638" s="16" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="639" spans="1:6" x14ac:dyDescent="0.25">
@@ -21707,7 +21704,7 @@
         <v>7</v>
       </c>
       <c r="F649" s="16" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
     </row>
     <row r="650" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -21727,7 +21724,7 @@
         <v>7</v>
       </c>
       <c r="F650" s="16" t="s">
-        <v>2637</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="651" spans="1:6" x14ac:dyDescent="0.25">
@@ -21787,7 +21784,7 @@
         <v>7</v>
       </c>
       <c r="F653" s="16" t="s">
-        <v>2638</v>
+        <v>2637</v>
       </c>
     </row>
     <row r="654" spans="1:6" x14ac:dyDescent="0.25">
@@ -21907,7 +21904,7 @@
         <v>7</v>
       </c>
       <c r="F659" s="16" t="s">
-        <v>2639</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="660" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -22067,7 +22064,7 @@
         <v>318</v>
       </c>
       <c r="F667" s="16" t="s">
-        <v>2661</v>
+        <v>2660</v>
       </c>
     </row>
     <row r="668" spans="1:6" x14ac:dyDescent="0.25">
@@ -22227,7 +22224,7 @@
         <v>620</v>
       </c>
       <c r="F675" s="16" t="s">
-        <v>2633</v>
+        <v>2632</v>
       </c>
     </row>
     <row r="676" spans="1:6" x14ac:dyDescent="0.25">
@@ -22347,7 +22344,7 @@
         <v>7</v>
       </c>
       <c r="F681" s="16" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
     </row>
     <row r="682" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -22687,7 +22684,7 @@
         <v>11</v>
       </c>
       <c r="F698" s="16" t="s">
-        <v>2638</v>
+        <v>2637</v>
       </c>
     </row>
     <row r="699" spans="1:6" x14ac:dyDescent="0.25">
@@ -23247,7 +23244,7 @@
         <v>7</v>
       </c>
       <c r="F726" s="16" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
     </row>
     <row r="727" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -23267,7 +23264,7 @@
         <v>7</v>
       </c>
       <c r="F727" s="16" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
     </row>
     <row r="728" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -23287,7 +23284,7 @@
         <v>7</v>
       </c>
       <c r="F728" s="16" t="s">
-        <v>2634</v>
+        <v>2633</v>
       </c>
     </row>
     <row r="729" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -23327,7 +23324,7 @@
         <v>7</v>
       </c>
       <c r="F730" s="16" t="s">
-        <v>2680</v>
+        <v>2679</v>
       </c>
     </row>
     <row r="731" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -23347,7 +23344,7 @@
         <v>7</v>
       </c>
       <c r="F731" s="16" t="s">
-        <v>2662</v>
+        <v>2661</v>
       </c>
     </row>
     <row r="732" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -23527,7 +23524,7 @@
         <v>7</v>
       </c>
       <c r="F740" s="16" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
     </row>
     <row r="741" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -23547,7 +23544,7 @@
         <v>7</v>
       </c>
       <c r="F741" s="16" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="742" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -23567,7 +23564,7 @@
         <v>7</v>
       </c>
       <c r="F742" s="16" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
     </row>
     <row r="743" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -23587,7 +23584,7 @@
         <v>7</v>
       </c>
       <c r="F743" s="16" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
     </row>
     <row r="744" spans="1:6" x14ac:dyDescent="0.25">
@@ -23887,7 +23884,7 @@
         <v>74</v>
       </c>
       <c r="F758" s="16" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="759" spans="1:6" x14ac:dyDescent="0.25">
@@ -23987,7 +23984,7 @@
         <v>175</v>
       </c>
       <c r="F763" s="16" t="s">
-        <v>2681</v>
+        <v>2680</v>
       </c>
     </row>
     <row r="764" spans="1:6" x14ac:dyDescent="0.25">
@@ -26507,7 +26504,7 @@
         <v>624</v>
       </c>
       <c r="F889" s="6" t="s">
-        <v>2645</v>
+        <v>2644</v>
       </c>
     </row>
     <row r="890" spans="1:6" x14ac:dyDescent="0.25">
@@ -26527,7 +26524,7 @@
         <v>87</v>
       </c>
       <c r="F890" s="6" t="s">
-        <v>2646</v>
+        <v>2645</v>
       </c>
     </row>
     <row r="891" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -26547,7 +26544,7 @@
         <v>206</v>
       </c>
       <c r="F891" s="6" t="s">
-        <v>2647</v>
+        <v>2646</v>
       </c>
     </row>
     <row r="892" spans="1:6" x14ac:dyDescent="0.25">
@@ -26587,7 +26584,7 @@
         <v>150</v>
       </c>
       <c r="F893" s="6" t="s">
-        <v>2648</v>
+        <v>2647</v>
       </c>
     </row>
     <row r="894" spans="1:6" x14ac:dyDescent="0.25">
@@ -26627,7 +26624,7 @@
         <v>626</v>
       </c>
       <c r="F895" s="6" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
     </row>
     <row r="896" spans="1:6" x14ac:dyDescent="0.25">
@@ -26667,7 +26664,7 @@
         <v>628</v>
       </c>
       <c r="F897" s="6" t="s">
-        <v>2650</v>
+        <v>2649</v>
       </c>
     </row>
     <row r="898" spans="1:6" x14ac:dyDescent="0.25">
@@ -26967,7 +26964,7 @@
         <v>633</v>
       </c>
       <c r="F912" s="16" t="s">
-        <v>2651</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="913" spans="1:6" x14ac:dyDescent="0.25">
@@ -26987,7 +26984,7 @@
         <v>87</v>
       </c>
       <c r="F913" s="16" t="s">
-        <v>2651</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="914" spans="1:6" x14ac:dyDescent="0.25">
@@ -27247,7 +27244,7 @@
         <v>634</v>
       </c>
       <c r="F926" s="16" t="s">
-        <v>2652</v>
+        <v>2651</v>
       </c>
     </row>
     <row r="927" spans="1:6" x14ac:dyDescent="0.25">
@@ -27267,7 +27264,7 @@
         <v>634</v>
       </c>
       <c r="F927" s="16" t="s">
-        <v>2652</v>
+        <v>2651</v>
       </c>
     </row>
     <row r="928" spans="1:6" x14ac:dyDescent="0.25">
@@ -27347,7 +27344,7 @@
         <v>7</v>
       </c>
       <c r="F931" s="16" t="s">
-        <v>2653</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="932" spans="1:6" x14ac:dyDescent="0.25">
@@ -27567,7 +27564,7 @@
         <v>7</v>
       </c>
       <c r="F942" s="16" t="s">
-        <v>2654</v>
+        <v>2653</v>
       </c>
     </row>
     <row r="943" spans="1:6" x14ac:dyDescent="0.25">
@@ -27760,8 +27757,8 @@
       <c r="C952" s="16" t="s">
         <v>835</v>
       </c>
-      <c r="D952" s="16" t="s">
-        <v>2628</v>
+      <c r="D952" s="16">
+        <v>0</v>
       </c>
       <c r="E952" s="16" t="s">
         <v>297</v>
@@ -27787,7 +27784,7 @@
         <v>171</v>
       </c>
       <c r="F953" s="16" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="954" spans="1:6" x14ac:dyDescent="0.25">
@@ -27807,7 +27804,7 @@
         <v>557</v>
       </c>
       <c r="F954" s="16" t="s">
-        <v>2632</v>
+        <v>2631</v>
       </c>
     </row>
     <row r="955" spans="1:6" x14ac:dyDescent="0.25">
@@ -28107,7 +28104,7 @@
         <v>22</v>
       </c>
       <c r="F969" s="16" t="s">
-        <v>2655</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="970" spans="1:6" x14ac:dyDescent="0.25">
@@ -28127,7 +28124,7 @@
         <v>45</v>
       </c>
       <c r="F970" s="16" t="s">
-        <v>2655</v>
+        <v>2654</v>
       </c>
     </row>
     <row r="971" spans="1:6" x14ac:dyDescent="0.25">
@@ -28287,7 +28284,7 @@
         <v>611</v>
       </c>
       <c r="F978" s="16" t="s">
-        <v>2656</v>
+        <v>2655</v>
       </c>
     </row>
     <row r="979" spans="1:6" x14ac:dyDescent="0.25">
@@ -28401,7 +28398,7 @@
         <v>808</v>
       </c>
       <c r="D984" s="16" t="s">
-        <v>2629</v>
+        <v>2628</v>
       </c>
       <c r="E984" s="16" t="s">
         <v>643</v>
@@ -28601,7 +28598,7 @@
         <v>156</v>
       </c>
       <c r="D994" s="16" t="s">
-        <v>2630</v>
+        <v>2629</v>
       </c>
       <c r="E994" s="16" t="s">
         <v>639</v>
@@ -28687,7 +28684,7 @@
         <v>19</v>
       </c>
       <c r="F998" s="18" t="s">
-        <v>2657</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="999" spans="1:6" ht="36" x14ac:dyDescent="0.25">
@@ -28821,7 +28818,7 @@
         <v>858</v>
       </c>
       <c r="D1005" s="18" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
       <c r="E1005" s="18" t="s">
         <v>171</v>
@@ -28987,7 +28984,7 @@
         <v>317</v>
       </c>
       <c r="F1013" s="18" t="s">
-        <v>2658</v>
+        <v>2657</v>
       </c>
     </row>
     <row r="1014" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -29147,7 +29144,7 @@
         <v>122</v>
       </c>
       <c r="F1021" s="18" t="s">
-        <v>2659</v>
+        <v>2658</v>
       </c>
     </row>
     <row r="1022" spans="1:6" ht="24" x14ac:dyDescent="0.25">
@@ -29316,6 +29313,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="מסמך" ma:contentTypeID="0x0101009B8A10DB9F21224B8EA1109F8E1C5334" ma:contentTypeVersion="4" ma:contentTypeDescription="צור מסמך חדש." ma:contentTypeScope="" ma:versionID="00463e6563a8385a95b25ed9e5224ff1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="39982820-3d8f-49d8-ba02-11f9eba628fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7df525748188a79234ce8ca095b02bf7" ns3:_="">
     <xsd:import namespace="39982820-3d8f-49d8-ba02-11f9eba628fc"/>
@@ -29461,22 +29473,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CE0B1E4-978F-4FFB-A3C8-2AE45350CDB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="39982820-3d8f-49d8-ba02-11f9eba628fc"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35CACD3F-96D1-4769-A6A2-4335C4F13F35}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A92D7097-6A92-4BF5-B4A8-A8A6133084BE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -29492,28 +29513,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35CACD3F-96D1-4769-A6A2-4335C4F13F35}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0CE0B1E4-978F-4FFB-A3C8-2AE45350CDB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="39982820-3d8f-49d8-ba02-11f9eba628fc"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>